<commit_message>
added more dynamic schedule readings
</commit_message>
<xml_diff>
--- a/assignment4/HeatForOMP/outputs/data.xlsx
+++ b/assignment4/HeatForOMP/outputs/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t xml:space="preserve">Threads</t>
   </si>
@@ -28,13 +28,19 @@
     <t xml:space="preserve">Static</t>
   </si>
   <si>
-    <t xml:space="preserve">Dynamic</t>
+    <t xml:space="preserve">Dynamic (4)</t>
   </si>
   <si>
     <t xml:space="preserve">Guided</t>
   </si>
   <si>
     <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic (70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dynamic (64)</t>
   </si>
   <si>
     <t xml:space="preserve">Single Core</t>
@@ -48,11 +54,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -71,6 +78,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -154,7 +166,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -182,7 +194,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF83CAFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
@@ -207,7 +219,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -371,7 +383,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dynamic</c:v>
+                  <c:v>Dynamic (4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -713,11 +725,245 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="32297272"/>
-        <c:axId val="53705157"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic (70)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.000" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$17:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$17:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.687930197406499</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.32829555674339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.37044064807489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.88569386270723</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.89381550387207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.87920912494244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.81586057689954</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.15763569939256</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1682093677884</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dynamic (64)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="83caff"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="0.000" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$17:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.688045386698305</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.33212650718191</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.37287523871984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.87972077679915</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8831412583978</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.87501468049007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.82420328382316</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.09137137065946</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.16354852717667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="75311121"/>
+        <c:axId val="19328954"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="32297272"/>
+        <c:axId val="75311121"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +993,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Threads</a:t>
+                  <a:t>Resolution</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -782,12 +1028,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53705157"/>
+        <c:crossAx val="19328954"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53705157"/>
+        <c:axId val="19328954"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +1098,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32297272"/>
+        <c:crossAx val="75311121"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -910,10 +1156,10 @@
       <xdr:rowOff>36360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>131760</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -922,7 +1168,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="36000" y="4100040"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="7605000" cy="4277520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -940,15 +1186,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,6 +1215,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -984,6 +1238,12 @@
       <c r="E2" s="1" t="n">
         <v>1.660628</v>
       </c>
+      <c r="F2" s="1" t="n">
+        <v>1.672488</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>1.672208</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1001,6 +1261,12 @@
       <c r="E3" s="1" t="n">
         <v>0.854887</v>
       </c>
+      <c r="F3" s="1" t="n">
+        <v>0.866189</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>0.863698</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1018,6 +1284,12 @@
       <c r="E4" s="1" t="n">
         <v>0.475883</v>
       </c>
+      <c r="F4" s="1" t="n">
+        <v>0.485376</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0.484878</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1035,6 +1307,12 @@
       <c r="E5" s="1" t="n">
         <v>0.396427</v>
       </c>
+      <c r="F5" s="1" t="n">
+        <v>0.39871</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>0.399537</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1052,6 +1330,12 @@
       <c r="E6" s="1" t="n">
         <v>0.399062</v>
       </c>
+      <c r="F6" s="1" t="n">
+        <v>0.397591</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.399063</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1069,6 +1353,12 @@
       <c r="E7" s="1" t="n">
         <v>0.402818</v>
       </c>
+      <c r="F7" s="1" t="n">
+        <v>0.399608</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.400191</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1086,6 +1376,12 @@
       <c r="E8" s="1" t="n">
         <v>0.413458</v>
       </c>
+      <c r="F8" s="1" t="n">
+        <v>0.408598</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.407391</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1103,6 +1399,12 @@
       <c r="E9" s="1" t="n">
         <v>0.286406</v>
       </c>
+      <c r="F9" s="1" t="n">
+        <v>0.276733</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>0.281215</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1120,10 +1422,16 @@
       <c r="E10" s="1" t="n">
         <v>0.286148</v>
       </c>
+      <c r="F10" s="1" t="n">
+        <v>0.276031</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0.27634</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1.150555</v>
@@ -1145,6 +1453,12 @@
       <c r="E16" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1166,6 +1480,14 @@
         <f aca="false">$B$13/E2</f>
         <v>0.692843309880358</v>
       </c>
+      <c r="F17" s="2" t="n">
+        <f aca="false">$B$13/F2</f>
+        <v>0.687930197406499</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <f aca="false">$B$13/G2</f>
+        <v>0.688045386698305</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1187,6 +1509,14 @@
         <f aca="false">$B$13/E3</f>
         <v>1.34585623597037</v>
       </c>
+      <c r="F18" s="2" t="n">
+        <f aca="false">$B$13/F3</f>
+        <v>1.32829555674339</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <f aca="false">$B$13/G3</f>
+        <v>1.33212650718191</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1208,6 +1538,14 @@
         <f aca="false">$B$13/E4</f>
         <v>2.41772662608246</v>
       </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">$B$13/F4</f>
+        <v>2.37044064807489</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <f aca="false">$B$13/G4</f>
+        <v>2.37287523871984</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1229,6 +1567,14 @@
         <f aca="false">$B$13/E5</f>
         <v>2.90231240556269</v>
       </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">$B$13/F5</f>
+        <v>2.88569386270723</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <f aca="false">$B$13/G5</f>
+        <v>2.87972077679915</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1250,6 +1596,14 @@
         <f aca="false">$B$13/E6</f>
         <v>2.88314848319309</v>
       </c>
+      <c r="F21" s="2" t="n">
+        <f aca="false">$B$13/F6</f>
+        <v>2.89381550387207</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <f aca="false">$B$13/G6</f>
+        <v>2.8831412583978</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -1271,6 +1625,14 @@
         <f aca="false">$B$13/E7</f>
         <v>2.85626511228396</v>
       </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">$B$13/F7</f>
+        <v>2.87920912494244</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <f aca="false">$B$13/G7</f>
+        <v>2.87501468049007</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -1292,6 +1654,14 @@
         <f aca="false">$B$13/E8</f>
         <v>2.78276148967973</v>
       </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">$B$13/F8</f>
+        <v>2.81586057689954</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <f aca="false">$B$13/G8</f>
+        <v>2.82420328382316</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -1313,6 +1683,14 @@
         <f aca="false">$B$13/E9</f>
         <v>4.01721681808342</v>
       </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false">$B$13/F9</f>
+        <v>4.15763569939256</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <f aca="false">$B$13/G9</f>
+        <v>4.09137137065946</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -1333,6 +1711,14 @@
       <c r="E25" s="2" t="n">
         <f aca="false">$B$13/E10</f>
         <v>4.0208388666005</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">$B$13/F10</f>
+        <v>4.1682093677884</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <f aca="false">$B$13/G10</f>
+        <v>4.16354852717667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>